<commit_message>
Added team meeting to my task log
yeah im lazy
</commit_message>
<xml_diff>
--- a/PSDs/Fetus/TaskList_FionaCheung.xlsx
+++ b/PSDs/Fetus/TaskList_FionaCheung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Day</t>
   </si>
@@ -71,16 +71,29 @@
   <si>
     <t>Made a quick blockout using 3D models I made earlier along with some new ones to get a feel for what the arena would look like.</t>
   </si>
+  <si>
+    <t>20.08.2021</t>
+  </si>
+  <si>
+    <t>Discussed what we've done over the past couple of days and what we plan to implement before we show the prototype to the lecturers next week.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -235,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -293,17 +306,6 @@
       <bottom style="thin">
         <color rgb="FFB7B7B7"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB7B7B7"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB7B7B7"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -382,68 +384,75 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -452,83 +461,79 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -536,7 +541,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -693,14 +706,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Sheet1-style" pivot="0" count="4">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="Sheet1-style 2" pivot="0" count="2">
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -721,13 +734,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:E75" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:E75" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <tableColumns count="5">
-    <tableColumn id="1" name="Day" dataDxfId="4"/>
-    <tableColumn id="2" name="Task name" dataDxfId="3"/>
-    <tableColumn id="3" name="What the task entails" dataDxfId="2"/>
-    <tableColumn id="4" name="1" dataDxfId="1"/>
-    <tableColumn id="5" name="Actual hours" dataDxfId="0"/>
+    <tableColumn id="1" name="Day" dataDxfId="5"/>
+    <tableColumn id="2" name="Task name" dataDxfId="4"/>
+    <tableColumn id="3" name="What the task entails" dataDxfId="3"/>
+    <tableColumn id="4" name="1" dataDxfId="2"/>
+    <tableColumn id="5" name="Actual hours" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -933,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -966,13 +979,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="13">
@@ -983,13 +996,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14">
@@ -1000,13 +1013,13 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="77" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="14">
@@ -1015,13 +1028,13 @@
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="77" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="14">
@@ -1029,108 +1042,118 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="15"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="15"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="14"/>
-      <c r="B9" s="22"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="15"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="23"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="20"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="27"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="27"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="30"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="14"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="G20" s="1"/>
@@ -1138,8 +1161,8 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="14"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="G21" s="1"/>
@@ -1147,395 +1170,395 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="14"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="31"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="30"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="31"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="35"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="38"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="G26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="38"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="G27" s="1"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="38"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="38"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="38"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="42"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="42"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="42"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="42"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="43"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="42"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="42"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="42"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="48"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="52"/>
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="54"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="52"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="54"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="52"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="54"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="52"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="51"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="54"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="52"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="54"/>
-      <c r="B44" s="53"/>
-      <c r="C44" s="52"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="54"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="52"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="52"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="51"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="52"/>
+      <c r="A47" s="57"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="51"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="58"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="52"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="51"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="58"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="58"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="56"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="19"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="58"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="63"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="62"/>
       <c r="D51" s="14"/>
-      <c r="E51" s="19"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="58"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="64"/>
-      <c r="B53" s="62"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
+      <c r="A53" s="63"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="64"/>
-      <c r="B54" s="60"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
+      <c r="A54" s="63"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="64"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
+      <c r="A55" s="63"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="64"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="58"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="64"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
+      <c r="A57" s="63"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="64"/>
-      <c r="B58" s="60"/>
-      <c r="C58" s="61"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
+      <c r="A58" s="63"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="65"/>
-      <c r="B59" s="66"/>
-      <c r="C59" s="67"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
+      <c r="A59" s="64"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="65"/>
-      <c r="B60" s="66"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="65"/>
-      <c r="E60" s="65"/>
+      <c r="A60" s="64"/>
+      <c r="B60" s="65"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="65"/>
-      <c r="B61" s="66"/>
-      <c r="C61" s="67"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
+      <c r="A61" s="64"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="65"/>
-      <c r="B62" s="66"/>
-      <c r="C62" s="67"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
+      <c r="A62" s="64"/>
+      <c r="B62" s="65"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="65"/>
-      <c r="B63" s="66"/>
-      <c r="C63" s="67"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
+      <c r="A63" s="64"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="65"/>
-      <c r="B64" s="66"/>
-      <c r="C64" s="67"/>
-      <c r="D64" s="65"/>
-      <c r="E64" s="65"/>
+      <c r="A64" s="64"/>
+      <c r="B64" s="65"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="65"/>
-      <c r="B65" s="66"/>
-      <c r="C65" s="67"/>
-      <c r="D65" s="65"/>
-      <c r="E65" s="65"/>
+      <c r="A65" s="64"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="65"/>
-      <c r="B66" s="66"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="65"/>
+      <c r="A66" s="64"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="65"/>
-      <c r="B67" s="66"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="65"/>
-      <c r="E67" s="65"/>
+      <c r="A67" s="64"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="65"/>
-      <c r="B68" s="66"/>
-      <c r="C68" s="67"/>
-      <c r="D68" s="65"/>
-      <c r="E68" s="65"/>
+      <c r="A68" s="64"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="65"/>
-      <c r="B69" s="66"/>
-      <c r="C69" s="67"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
+      <c r="A69" s="64"/>
+      <c r="B69" s="65"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="65"/>
-      <c r="B70" s="66"/>
-      <c r="C70" s="67"/>
-      <c r="D70" s="65"/>
-      <c r="E70" s="65"/>
+      <c r="A70" s="64"/>
+      <c r="B70" s="65"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="65"/>
-      <c r="B71" s="66"/>
-      <c r="C71" s="67"/>
-      <c r="D71" s="65"/>
-      <c r="E71" s="65"/>
+      <c r="A71" s="64"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="65"/>
-      <c r="B72" s="66"/>
-      <c r="C72" s="67"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
+      <c r="A72" s="64"/>
+      <c r="B72" s="65"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="65"/>
-      <c r="B73" s="66"/>
-      <c r="C73" s="67"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
+      <c r="A73" s="64"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="68"/>
-      <c r="B74" s="69"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="67"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="71"/>
-      <c r="B75" s="72"/>
-      <c r="C75" s="70"/>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
+      <c r="A75" s="70"/>
+      <c r="B75" s="71"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="67"/>
+      <c r="E75" s="67"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1">
       <c r="A76" s="9" t="s">
@@ -1545,11 +1568,11 @@
       <c r="C76" s="6"/>
       <c r="D76" s="6">
         <f>SUM(Sheet1!$D$2:$D$75)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E76" s="10">
         <f>SUM(Sheet1!$E$2:$E$75)</f>
-        <v>4.88</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1">
@@ -2507,8 +2530,8 @@
     <row r="1015" ht="15.75" customHeight="1"/>
     <row r="1016" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="H23:H27 C25:C28 C2:C18 B4:C4 B2:B28 B28:C75">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="1">
+  <conditionalFormatting sqref="H23:H27 C25:C28 C2:C18 B4:C4 B28:C75 B2:B28">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
We now have an application icon
</commit_message>
<xml_diff>
--- a/PSDs/Fetus/TaskList_FionaCheung.xlsx
+++ b/PSDs/Fetus/TaskList_FionaCheung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Day</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Tweaked start screen title placement and size. Also updated 3D backdrop with Roger's new scene.</t>
+  </si>
+  <si>
+    <t>Custom Title</t>
+  </si>
+  <si>
+    <t>Made a custom title based off Fenrir Regular.</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -595,9 +601,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -741,6 +744,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1199,13 +1206,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="13">
@@ -1216,13 +1223,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="14">
@@ -1233,13 +1240,13 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="14">
@@ -1250,13 +1257,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="14">
@@ -1267,50 +1274,50 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="61">
         <v>1</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="61">
         <v>0.73</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="61">
         <v>1</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="61">
         <v>0.52</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="61">
         <v>1</v>
       </c>
       <c r="E8" s="14">
@@ -1318,13 +1325,13 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="78" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="14">
@@ -1335,13 +1342,13 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="68" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="14">
@@ -1352,13 +1359,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="14">
@@ -1369,13 +1376,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="70" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="14">
@@ -1386,13 +1393,13 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="70" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="14">
@@ -1403,13 +1410,13 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="14">
@@ -1420,13 +1427,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="14">
@@ -1437,13 +1444,13 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="14">
@@ -1454,13 +1461,13 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="75" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="14">
@@ -1471,13 +1478,13 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="76" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="14">
@@ -1488,13 +1495,13 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="75" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="14">
@@ -1505,13 +1512,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="75" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="14">
@@ -1524,13 +1531,13 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="81" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="14">
@@ -1543,13 +1550,13 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="81" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="14">
@@ -1562,13 +1569,13 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="30">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="85" t="s">
+      <c r="C23" s="84" t="s">
         <v>55</v>
       </c>
       <c r="D23" s="14">
@@ -1581,13 +1588,13 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="30">
-      <c r="A24" s="83" t="s">
+      <c r="A24" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="85" t="s">
         <v>59</v>
       </c>
       <c r="D24" s="14">
@@ -1600,13 +1607,13 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="86" t="s">
         <v>58</v>
       </c>
       <c r="D25" s="14">
@@ -1619,13 +1626,13 @@
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="85" t="s">
         <v>60</v>
       </c>
       <c r="D26" s="14">
@@ -1638,13 +1645,13 @@
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="83" t="s">
+      <c r="A27" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="85" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="14">
@@ -1657,13 +1664,13 @@
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="89" t="s">
+      <c r="C28" s="88" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="14">
@@ -1676,11 +1683,21 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="18"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="18"/>
@@ -1690,319 +1707,319 @@
       <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="23"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="22"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="22"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="23"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="26"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="22"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="32"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="31"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="34"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="32"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="31"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="34"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="32"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="31"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="34"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="32"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="31"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="34"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="32"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="31"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="34"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="32"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="31"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="34"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="32"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="31"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="38"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="32"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="31"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="38"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="32"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="31"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="38"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="32"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="31"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="38"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="38"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="36"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="14"/>
       <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="38"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="43"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="42"/>
       <c r="D51" s="14"/>
       <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="38"/>
-      <c r="B52" s="42"/>
-      <c r="C52" s="43"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="44"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
+      <c r="A53" s="43"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="44"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="44"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="44"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="44"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="44"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="45"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="45"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="45"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="45"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="45"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="45"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="45"/>
-      <c r="B64" s="46"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="45"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="45"/>
-      <c r="B65" s="46"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="45"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="45"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="47"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="45"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="45"/>
-      <c r="B68" s="46"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="45"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="45"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="45"/>
-      <c r="B70" s="46"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="45"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="45"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
+      <c r="A71" s="44"/>
+      <c r="B71" s="45"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="45"/>
-      <c r="B72" s="46"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
+      <c r="A72" s="44"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="45"/>
-      <c r="B73" s="46"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
+      <c r="A73" s="44"/>
+      <c r="B73" s="45"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="48"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="51"/>
-      <c r="B75" s="52"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
+      <c r="A75" s="50"/>
+      <c r="B75" s="51"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1">
       <c r="A76" s="9" t="s">
@@ -2012,11 +2029,11 @@
       <c r="C76" s="6"/>
       <c r="D76" s="6">
         <f>SUM(Sheet1!$D$2:$D$75)</f>
-        <v>21.400000000000002</v>
+        <v>21.500000000000004</v>
       </c>
       <c r="E76" s="10">
         <f>SUM(Sheet1!$E$2:$E$75)</f>
-        <v>22.090000000000003</v>
+        <v>22.370000000000005</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>